<commit_message>
Comment out unnecessary log messages for Append .NET/JAVA .xaml
</commit_message>
<xml_diff>
--- a/Trello Backlog Dispatcher/Trainer Name List.xlsx
+++ b/Trello Backlog Dispatcher/Trainer Name List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <x:si>
     <x:t>Board ID</x:t>
   </x:si>
@@ -28,19 +28,22 @@
     <x:t>Board Name</x:t>
   </x:si>
   <x:si>
-    <x:t>62b8c15c015f476779a11a2c</x:t>
+    <x:t>62b8ebddeb5f78389b68cbbf</x:t>
   </x:si>
   <x:si>
     <x:t>Andrew Shields-Java Foundations Project</x:t>
   </x:si>
   <x:si>
-    <x:t>62b8c15cf245272a7ce4713f</x:t>
+    <x:t>62b8d257b8f7598718367a01</x:t>
   </x:si>
   <x:si>
     <x:t>Marielle Nolasco-.NET Foundations Project</x:t>
   </x:si>
   <x:si>
-    <x:t>62b8c15ca3f5b080b9a8c4da</x:t>
+    <x:t>62b8ebddcf728a4dbd624d11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62b8ebdd5226315c99f9b256</x:t>
   </x:si>
   <x:si>
     <x:t>Moiya Josephs-Java Foundations Project</x:t>
@@ -443,7 +446,7 @@
       <x:selection activeCell="A1" sqref="A1 A1:A1"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="50.619531" defaultRowHeight="12.8" zeroHeight="false"/>
+  <x:sheetFormatPr defaultColWidth="167.872656" defaultRowHeight="12.8" zeroHeight="false"/>
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" s="1" t="s">
@@ -475,7 +478,15 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B5" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2">
+      <x:c r="A6" s="1" t="s">
         <x:v>7</x:v>
+      </x:c>
+      <x:c r="B6" s="1" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>